<commit_message>
Get daily reddit data: Tue May  7 08:08:33 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_12.xlsx
+++ b/data/2024_05_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C455"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2624 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1cm6arn</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just bought glue so this wouldn’t happen 🥲 I don’t wanna cut them </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i04fdw70lyyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1cm60dl</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Purple time 💜</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm60dl</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1cm5w9h</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>OPI’s Malaga Wine with ILNP’s Ruby on top✨🩸</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdv3fbbpfyyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1cm5t8w</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Nail tech is showing off as usual</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biqsu8nleyyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1cm3tkb</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Help, are apropriate for a wedding?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7rw2f32rxyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1cm335p</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>tried nail sticker thingys for the first time, not too bad imo!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm335p</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1clfezi</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>vacation nails 🌺</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lakkg706syc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1clkoxk</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>My nail tech ate with this nude Russian manicure</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clkoxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1cll5w3</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Got a shellac manicure on Friday. One nail is lifting today. What can I do?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s4i4ch4mtyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1cllrl1</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Facebook swap groups? </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cllrl1/facebook_swap_groups/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1cm0grk</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>With clear press ons, how do I avoid the markings of the glue and tension from pressing down?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cm0grk/with_clear_press_ons_how_do_i_avoid_the_markings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1clprwn</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Monochromatic Nail Art</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zaosq2kjuyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1cltywx</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>How do I get rid of the hard white parts around my nails?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ca50s03aevyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1clwcb8</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Need some inspiration for a trip!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clwcb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1cm20oc</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>I love something as big and sharp as a cat's nails</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4gerjew8xyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1cm1x8q</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Help me buy a nail drill for my wife</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cm1x8q/help_me_buy_a_nail_drill_for_my_wife/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1cm1t6l</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what is the best fast drying top coat??? </t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cm1t6l/what_is_the_best_fast_drying_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1cm19qx</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Need help</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm19qx</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1cm0lhe</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Dream Gel?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/usq6idcbwwyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1cm0bd8</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>New Pedi</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f5xk1eutwyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1cm07d1</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>A wanted a touch of sparkle without them all being the same! What you think?!</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm07d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1clzrjb</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>I do my sister’s nails for practice. Any feedback?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clzrjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1clzppa</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Why did the metallic part lose its luster once I applied the top coat?</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxgdk9dkowyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1clzej7</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yea? </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yshji45vlwyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1clz04l</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Favorite Set So Far</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jx1mkr7iwyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1clz014</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>3 Polish Mani w/Thermal - Mooncat &amp; Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clz014</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1clyefz</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Nail day!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31hl557xcwyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1cly6n9</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Glow in the dark press ons!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cly6n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1clxnou</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>So shifty shifty</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clxnou</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1clxkpt</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>I’ve got the summer fever ☀️</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93izs6v16wyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1clxjg4</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I made this for myself ! Rate please ! </t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywzhizyq5wyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1clx0o1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Had to go back to the classics 🙂‍↕️ but i think them look better on squares</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clx0o1</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1clwurq</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My first nails</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clwurq</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1clvzqy</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone else hate dipping powder? </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clvzqy/does_anyone_else_hate_dipping_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1clvwmr</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Vampire Nails 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lozxv1cksvyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1cluspb</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>I'm just a girl ✨</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5710n7o9kvyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1clupu9</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Love my new spring nails!!🌸</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clupu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1clu1tc</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Marble Nails</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clu1tc</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1clts95</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>playoff nails!</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l68vgzlvcvyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1clto45</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>My cutest set yet! I started doing my own acrylics during the beginning of the pandemic and have come a long way since then. (Featuring uranium glass frog)</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clto45</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1cltesv</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Colored UV gel underneath transparent polygel?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cltesv/colored_uv_gel_underneath_transparent_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1clt6x3</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Bridal nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94zx4r4f8vyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1clsopc</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>First time using Glammetic press ons! These are my birthday nails and I love them!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clsopc</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1clsmr0</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Suggestions</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clsmr0/suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1clsdxn</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvhjqatm2vyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1cls151</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these press ons! </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h52bw7t20vyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1clakx8</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blank press ons </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clakx8/blank_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1clrmzy</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Spring whimsy 🧚</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yslpxfb5xuyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1clrhp4</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>mold or bruising?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clrhp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1clqrr2</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is Tricoci University a reputable nail school? </t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clqrr2/is_tricoci_university_a_reputable_nail_school/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1clqbr3</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Silver Chrome Almond Frenchies 😍</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clqbr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1clpk55</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>I want to grow out my natural nails, but i cant consistently wear any type of layer on my nails</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clpk55/i_want_to_grow_out_my_natural_nails_but_i_cant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1clp43f</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Nail stickers are so convenient</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w26nlvseuyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1clnyri</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>I painted nails inspired by Iso from Valorant</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clnyri</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1clo6sk</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>First time doing 3d flowers</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clo6sk</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1clnwmt</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>butterfly🦋🦋</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9fvzr416uyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1clnwjf</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>First set in years!</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qyser806uyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1clmgau</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy spring nails for todays client! </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vin0vqgjvtyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1clmg5e</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Any thing I can/should do for the lifting bit on the bottom left of my thumb nail on my gel soak offs?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a164n1fivtyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1cllzsr</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Why won’t my nail polish go on smooth? Both the color and clear polish I used are fairly new, bought within the past few months.</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cllzsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1cllzrf</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Nude nails with marble detail, first attempt!</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cllzrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1clllil</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on recommendations for big man hands? </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clllil/press_on_recommendations_for_big_man_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1clkz46</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Wide &amp; Curling nails, need advice!</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clkz46/wide_curling_nails_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1clk8n8</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Simple but with a different touch</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8jlp3983ftyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1clk2vn</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can i make my bad boys look nicer? </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du5vt4iudtyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1cljqv1</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Solar Polishes</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cljqv1</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1cljawk</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>This iridescent purple is my favorite color ever</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp2n4ftp7tyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1clj2z6</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>💜🦋 So happy with how these turned out !!</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yi2a2nfx5tyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1clisac</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Loving this set ❤️</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep2vrmmi3tyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1clirr6</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Chrome stars on my shorties✨</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1o5li5e3tyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1cliqzb</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Which nail shape??</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cliqzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1clhjki</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Anything I can do about this?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0azkvvjkssyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1clh2yv</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Loving this set! Gel on natural nails!</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqpt73o8osyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1clgvyg</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>looks very delicate to me</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clgvyg/looks_very_delicate_to_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1clgeot</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Cat eye blue silver and black base</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u724pvqchsyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1clg35q</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Opinion on clear nails ? I think they are so freaking cool, but many people find them weird? 🫤 😀(those are press ons)</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clg35q</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1clfxrn</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>The blue part reminds me of a sea wave</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1clfxrn/the_blue_part_reminds_me_of_a_sea_wave/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1clezog</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mavala Jodhpur </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p81e5pyp0syc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1clexof</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>How can I fix this nail and the skin above the nail ?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eb42ozl00syc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1cle9s2</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Finally did the chrome powder ornament thing, very in love 💕</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cle9s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1cldtb4</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Did my nails in the car, turned out okay 🙃</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/868gbz7rlryc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1cm5zti</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Purple time 💜</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm5zti</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1cm40wa</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Chameleon Cortana</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm40wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1cm3pac</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Guys is my nail ever going to be fixed???</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djkeuc9vpxyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1cm3a5v</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>LynB - My Hobby is Solving Murders</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm3a5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1cm32r3</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Nail growth Update</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm32r3</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1cm1u8k</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Is it weird I just push my cuticles back with my nails?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cm1u8k/is_it_weird_i_just_push_my_cuticles_back_with_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1cm1hw3</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>PSA Ether Dragon is coming back for PPU Rewind 🐉✨</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm1hw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1cm1btk</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Mileena Wins</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7qivauvp2xyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1cm0sbn</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>DND Blue Island, IL with white chrome powder</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm0sbn</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1clz40a</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>3 Polish Mani w/Thermal - Mooncat &amp; Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clz40a</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1cly8ey</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>ILNP Flower Child</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cly8ey</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1clm1qx</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for gift ideas! </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b1zdrhlstyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1clx81q</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Has anyone tried using a polish base coat under glue on nails? Did they last as well as glue applied directly to your natural nails?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clx81q/has_anyone_tried_using_a_polish_base_coat_under/</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1clwjbw</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I feel like I jumped into a lagoon</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clwjbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1clw1pb</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MC Artemis deathkiss vs CC deja vu </t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clw1pb/mc_artemis_deathkiss_vs_cc_deja_vu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1clvtyu</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Why are gel-like top coats in opaque bottles if they're not actually gel or need light to set/dry/cure?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clvtyu/why_are_gellike_top_coats_in_opaque_bottles_if/</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1clviqp</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Look Alive</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clviqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1clvifg</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Best Linear Holo Topper?</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clvifg/best_linear_holo_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1clv8jb</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Paid 110 and I’m unhappy with the results. Any advice?</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf0g5l2lnvyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1clv6ld</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Cosmic Chaos ☄️</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clv6ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1clv5s1</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>I *tried* to do butterfly nails 🦋💜</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ot13se0nvyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1cluxb3</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Love Spell by Holo Taco</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sicwkok7lvyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1cluv60</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Obsessed!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p10pub0skvyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1clusjg</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Pear-adise Cove by OPI</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nj5v9c8kvyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1clu4vn</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>My first ILNP polish 🪻</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clu4vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1clstmp</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Help ! Peeled thumb nails from press ons</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clstmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1clsmex</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Paint splatter and silver dots</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/pL0va3N</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1clsj4j</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>simple but so beautiful</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clsj4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1clsg0a</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Glow and Reflective Purples Paired</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clsg0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1clsbhf</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Day 11 of Mercurys Tears- no chips!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clsbhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1cls8bp</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Tried ombré. Made a mess. Rage quit. Tried again. Not perfect but making progress!</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cls8bp</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1clrquk</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t xml:space="preserve">something spring-like </t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clrquk</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1clrb7d</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Of course.</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clrb7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1clraev</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"Fishing" for compliments </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clraev</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1clr7hj</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Bluebell</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clr7hj</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1clpwmw</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Question for those of you who have been doing this for a while: are backup bottles a bad idea?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clpwmw/question_for_those_of_you_who_have_been_doing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1clpv93</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Candy Castle - LynBDesigns</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clpv93</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1clp68s</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Question for colors you don't like.</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clp68s/question_for_colors_you_dont_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1clp22m</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>A little late but I wanted to share my April manicures 😸</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clp22m</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1cloz8p</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>First DIY gel nails!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cloz8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1clooaz</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>My first holo and glitter polishes</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x82jckwlbuyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1clog3m</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Sometimes it's just a no, dawg.</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clog3m/sometimes_its_just_a_no_dawg/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1cloclo</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Skiing is Believing by KBshimmer</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cloclo</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1clnbg8</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>We have House of Hades at home!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y93pbp0q1uyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1clmxrm</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Regarding Witch's Ball and Black Dog</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clmxrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1clmki6</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>In love with Drunk Fairy Calliope</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clmki6</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1clm281</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Anyone else buy a shade mostly because of name/theme?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clm281</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1clls3l</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Facebook swap groups? </t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clls3l/facebook_swap_groups/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1clkry3</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Non Maniology stamping plates</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clkry3/non_maniology_stamping_plates/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1clkpp4</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Got a shellac mani on Friday and have lifting today. What can I do?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw2880bqityc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1clk6pk</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Feeling spicy 🌶️</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhqjwvqoetyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1cljxta</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Y’all already know what this color is</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cljxta</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1cljwik</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Messy dots 🫣</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/izlctlkfctyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1clhqha</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Free hand lemons on an impatient girlie (hence the smudge)</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/68arkeydusyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1clh1ta</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Kitchen sink-lite approach worked</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clh1ta</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1cl4t9z</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Molten Lava 🔥 </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xze43e1u0pyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1clfbem</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1clfbem/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1cm6f5t</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Press ons ︎︎𓂃⟡.·</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm6f5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1cm4t81</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Butterfly nails 💅</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm4t81</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1clzukc</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Red and Pearls ❤️</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m4q1vd5qpwyc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1clz5xs</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green Y2K Nails Inspired </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bjhfptojwyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1clxlwf</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I am finally starting to get better. Even though I can still pick out 1 million things wrong with these.</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yswv8jbb6wyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1clxcc0</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Supplies</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1clxcc0/supplies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1clvxp4</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Suggestions on getting started</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1clvxp4/suggestions_on_getting_started/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1clt3pt</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Did I ruin my nail stamping plates?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nedmpylr7vyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1cls3s1</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried some flowers today! </t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er6k829l0vyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1clpnr3</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Took 3 hours but worth it</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1clpnr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1clmu7s</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>How do my press ons look</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/okia02paytyc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1clma51</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Super proud of these ❤️🐍</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pjfvvz9utyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1cllxqw</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Did These To Match An Outfit And I'm Over The Moon With How They Came Out! ✨💞🌙</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cllxqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1clj3j9</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>💜🦋 So happy with how these turned out !!</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb6d5si26tyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1clik4x</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Nails, ft. Decent Cuticles</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na5q57co1tyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1clghyu</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Latest set cat eye blue over black base</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrs9t59cisyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed May  8 08:07:54 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_12.xlsx
+++ b/data/2024_05_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C455"/>
+  <dimension ref="A1:C610"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8168,6 +8168,2641 @@
         </is>
       </c>
     </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1cmx1uz</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>kitten bit a hole through my nail bed</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3of5b26735zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1cmvths</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>How do y’all function with this kind of nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0nixuvtp4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1cmvsmw</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Jello Jello One Kill Peel Off Price</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmvsmw/jello_jello_one_kill_peel_off_price/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1cmvr2d</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>does this colour suit my skin tone ?</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxeuc4d4p4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1cmvi7c</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>The way I’m obsessed with them 🩵 just got em done yesterday 🩵🩵</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmykg8fpm4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1cmvesh</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Please explain these color shifting nails to an ignorant 70 year old male</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmvesh/please_explain_these_color_shifting_nails_to_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1cmv71q</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>First time doing brushwork! I'm pleased with the result, C&amp;C welcome</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmv71q</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1cmv06s</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done for the first time in 2ish years. Very happy to have a French mani back. </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24mn5wjth4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1cmuwh9</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Will I ever have nice nails?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqzlbgntg4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1cmupnl</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Periwinkle chrome gel nails</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fz6aupy1f4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1cmu0e5</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Milky white 🤤</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psd6d53m84zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1cmtga7</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Nail tech went all out for my birthday :)</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmtga7</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1cmtfm6</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Any critics</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmtfm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1cmtemo</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Just finished this hand! Onto the next one.. Tomorrow</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3iajl32534zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1cmtb4p</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Good matte coatings?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmtb4p/good_matte_coatings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1cmt9nz</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Hangnail looking thing? What is it and what should I do to get rid?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmt9nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1cmt74q</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Dual form nails with hard gel</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmt74q</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1cmt0g8</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Been a while since I got my nails done</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m36mrurrz3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1cmsqe6</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>New set 🌸🌸🌸</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmsqe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1cmsp21</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Extra short are still too long for my nails!</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmsp21</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1cmsnk9</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>First time i left me this size of nails and I feel that it’s my new era and the color is very top</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xywe1yqkw3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1cmsj4u</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>got my  nails down</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eslmxe9gv3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1cms109</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>I usually don’t see to many pedicure posts but I LOVE my moo cow piggies</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2e6fsovq3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1cmrxaz</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>I love them this short, I got used to this size and now I don't want to have them long again.</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/uuxa3zD.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1cmrfal</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>New nails 💅🏽😘</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmrfal</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1cmqw98</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Witch nails?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmqw98</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1cmqkwh</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Not the greatest lighting but wanted to share</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7zmr4b0e3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1cmq9c2</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Haven’t done my nails in a while </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uerho9ebb3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1cmq5pm</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>thoughts on this color palette?</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmq5pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1cmpmy2</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Flowery Nails!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opjvqqu663zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1cmpgkp</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Spring nails 💅</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xki4sift43zc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1cmp8j2</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>First attempt at chrome nails</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmp8j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1cmp1en</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>i really like my polly pocket nails💕</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmp1en</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1cmos2c</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>New nudes 🫧</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ptcmykkz2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1cmokd8</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Half moon nails!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmokd8</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1cmoj8b</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>In the clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmoj8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1cmodu3</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Best UV/LED lamps in UK?</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmodu3/best_uvled_lamps_in_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1cmoagv</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today Nails </t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxzwzupzv2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1cmnl7w</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail artist has been booked up. I finally go this weekend. Its been 5 weeks 😵‍💫 </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cybphohsq2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1cmniwc</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Just finished my vacation nails!</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmniwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1cmmfru</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Left my cooking job to go back to school so I had to get my nails done to celebrate!</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edya49ydi2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1cm8atk</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>This will be my last straw. How do I stop it from breaking😭 The underside of the nail is still solid, the top is cracked</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muac4gwlazyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1cmayrg</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>First time doing Gel X Nails. When the extension fell off on 2 of the nails there ended up being a break in the shaft. Why could this happen and what should I do?</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkgyy5mb20zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1cmb1vx</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Sailor Moon nails</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmb1vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1cmcms5</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Allergic to gel</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmcms5/allergic_to_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1cmlvz9</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>I ❤️Press ons! Keepin it real simple</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmlvz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1cmdqs2</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Chrome Powder on Non-Gel Nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmdqs2/chrome_powder_on_nongel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1cmdwe2</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>My most favorite nails I’ve done on myself!</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsvodlxiq0zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1cmid2z</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kid-friendly! </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmid2z/kidfriendly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1cmltwe</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Naptime nails, pink spring flowers 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmltwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1cmlmgf</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Simple baby blue</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ubsc89gc2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1cmlkgs</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Spring nails :)</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8ge4vv1c2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1cml9eb</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Little flowers for the end of spring</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cml9eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1cmkpql</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hc89yzq52zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1cmkjq3</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hard gel vs gel overlay? </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmkjq3/hard_gel_vs_gel_overlay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1cmkd9t</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Opi private jet</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6cckzof532zc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1cmk7th</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Love these colors, Mani from 4/26</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmk7th</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1cmk61a</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>My nail art ✨</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmk61a</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1cmjvf6</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Still very new to the world of nails but happy with my 2nd attempt with gel 😊</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmjvf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1cmjiwz</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I love nail charms</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2r5aofcww1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1cmjcjb</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Springtime nails 🌸</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmjcjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1cmjc0f</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Done by me🥰 the pallet and the nails♥️ kinda reminds me of the zebra striped gum lol this set took me 6 hours</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmjc0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1cmhxhv</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>4th time diy-ing my nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmhxhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1cmhf9z</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Mint</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6qe4qq5h1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1cmh6oo</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>manicure for my graduation 😭😭😭</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf85ol9bf1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1cmgsui</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Summer in Florida</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otfe8i9gc1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1cmgpa6</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Newly obsessed with press/glue ons. Any advice to perfect the technique?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3cl6b2pb1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1cmgnsx</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>I’m new. I know application is crap it’s my second try! Need advice about shaping my nail beds</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aj5ta9db1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1cmghbd</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Zoya’s “Ali” is just what I need</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmghbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1cmgd5b</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>fresh self-done manicure on natural nails</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmgd5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1cmg5nd</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>My spring set 🌼 DIY hand painted, a holo nail, and some 3D</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmg5nd</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1cmg2ag</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Little fluffy clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/Cb0pMee.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1cmfl76</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seeing my sister's nails makes me want to cut them into a square shape. </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lifuzxx331zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1cmf48c</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">At home IBD hard gel nails :) </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmf48c</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1cmet2r</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Matte black and yellow!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/le5nbf3fx0zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1cmekzg</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Acrylic Refill over Biogel Artificial Nails?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmekzg/acrylic_refill_over_biogel_artificial_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1cmdxrr</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total neewb. </t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmdxrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1cmdw1h</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help for a newbie! </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmdw1h/help_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1cmdvza</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help for a newbie! </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmdvza/help_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1cmdpct</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Newest set</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmdpct</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1cmdh4c</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>I love my nails but not my hand 🫠</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8qx0ri6n0zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1cmd7km</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Impress nails</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmd7km</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1cmd5yp</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Nails popping off</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmd5yp</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1cmd4hn</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Trying something new</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g9n81nck0zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1cmcynx</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cow print </t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmcynx/cow_print/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1cmbjd5</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>My younger cousin did my nails, can’t get over how cute they are!</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmbjd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1cmadv4</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Im not great at doing my nails 🙈</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2070xdvwzyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1cmadd8</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY gel overlay- difficulty level </t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmadd8/diy_gel_overlay_difficulty_level/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1cma83x</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Florals? For spring? Groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7wcykkbvzyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1cm9pg2</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ink on BIAB </t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/piwej5m7qzyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1cm9hlz</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Barbie claws</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stm92a3ynzyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1cm8r0x</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Thoughts? 😊</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/816w7x0yfzyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1cm8q86</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Pretty proud of this one, still pretty new to nail art. Feedback is welcome!</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfbo5iymfzyc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1cm8hor</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>🦋🦋🦋</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm8hor</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1cm7ze6</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Jumping on the milky mani trend 🐮</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm7ze6</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1cm7ql8</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>No matter what I do my nails always split like this. I can't grow them out. I oil I moisturise and it still happens (sorry for the awkward photos but it's hard to take a photo of something so small😅)</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm7ql8</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1cm6zpe</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>delicate pattern and beautiful milky shade</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cm6zpe/delicate_pattern_and_beautiful_milky_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1cmyze6</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Jelly Nails 🍓</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81gfv2jpq5zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1cmxsew</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>In love with this skittle!</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62b5539vb5zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1cmwe05</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Gradient attempt</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twtq4biuv4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1cmw8q5</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Mooncat Cheshire Cat Dupe?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmw8q5/mooncat_cheshire_cat_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1cmvs8t</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Discord Drama: A Different POV</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmvs8t/discord_drama_a_different_pov/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1cmvms7</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Follow for more cute nails 🤍</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kbz6lhyn4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1cmuvik</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Reverie</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmuvik</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1cmuiya</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lumen Aurora Beam is so cute in low light </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/eao98ryad4zc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1cmtgzc</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>So 💔Disappointed</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmtgzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1cmsuy8</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>solo mission by holo taco 👽</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn2msj3ey3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1cmsqn2</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>So many compliments on this one</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmsqn2</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1cmsbck</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Is non-UV "gel" polish a thing? Especially when it concerns acrylates?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmsbck/is_nonuv_gel_polish_a_thing_especially_when_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1cmsawd</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>SUMMARY OF DISCORD DRAMA</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmsawd/summary_of_discord_drama/</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1cmrkjh</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>First reflective…do they all get this gritty textured finish?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmrkjh</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1cmrjm0</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>[meta] was the Reddit lacqueristas discord server just deleted?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmrjm0/meta_was_the_reddit_lacqueristas_discord_server/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1cmrgre</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Love Little Fox</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmrgre</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1cmqoac</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Jelly nails of my dreams</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvqzx1kue3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1cmpjq9</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>I wanted to love you</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmpjq9</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1cmo8ju</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t xml:space="preserve">does the poppy not fit olive and june’s polishes? </t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wv6ivglv2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1cmnrw3</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Orly Retrograde</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmnrw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1cmn7fu</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almost Monochromatic </t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmn7fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1cmn1l1</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>12 points to the Netherlands 🇳🇱</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j34yvfysm2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1cmn0po</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Simple little wintry look I did this past January :)</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmn0po</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1cmlqkd</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Regular polish dupes for these gels?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmlqkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1cmaf4f</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Mortals Be Warned vs Cygnus Loop</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmaf4f/mortals_be_warned_vs_cygnus_loop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1cmlduu</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>My friends hate the way I send manicure pictures</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vgrkflpa2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1cml4yg</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Spring pink flowers 🌸</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cml4yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1cmjrb1</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨️sparkle ✨️ </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmjrb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1cmjhez</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>My last 3 manis</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmjhez</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1cmioga</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Recommendations Needed!</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmioga/recommendations_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1cmi7cs</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>matches the 70 degree weather</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57tyfqc5n1zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1cmh4ub</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>I love jelly nail polish</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmh4ub</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1cmgl48</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>US Drugstore-accessible French manicure shades for Raynaud's sufferers?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmgl48/us_drugstoreaccessible_french_manicure_shades_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1cmgjod</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Are there any dupes for Mooncat's Ultrahot?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmgjod/are_there_any_dupes_for_mooncats_ultrahot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1cmfsel</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Favorite royal blue shimmer?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmfsel/favorite_royal_blue_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1cmfogy</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No more dubious used polish </t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5nwehjw31zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1cmfj37</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>I absolutely love the way this topcoat looks on bare nails</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dsrnu37r21zc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1cmf01g</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Mooncat Speed Demon vs INM Out The Door topcoat?</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmf01g/mooncat_speed_demon_vs_inm_out_the_door_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1cmeqlt</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Orly Star Fire</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmeqlt</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1cmepv0</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>✨️🧲Magnetic Sparkle🧲✨️</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmepv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1cmeia5</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Best UV/LED lamps in UK?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmeia5/best_uvled_lamps_in_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1cmdnpa</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>how to fix damaged nails from digging underneath them?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4vztt2no0zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1cmdap9</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Mother’s Day Help!</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmdap9/mothers_day_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1cmc2u9</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Cozy spring</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atjldic0c0zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1cmalsm</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>BKL — I’ll devour all of you</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmalsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1cmupvy</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Nails for my short film 🌙✨</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bxedbp3f4zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1cmqxs3</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>blue press on nails 🩵</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ppvufi2h3zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1cmqfpb</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>black frenchies</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmqfpb</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1cmq5nl</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Red and gold design I did ✨</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmq5nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1cmo0sp</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvxun37zt2zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1cmnwgi</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Nails I did for my SIL</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmnwgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1cmlupd</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Nail art novice but I love a dot flower 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmlupd</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1cmj2o7</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Simple and white</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmj2o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1cmiunq</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Painted as a birthday present for my mum</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tylk8pyr1zc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1cmijpy</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Birthday nails for my sister</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oipvj7fop1zc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1cmdem6</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Flowers </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmdem6</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1cm9sgu</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Buu nails!</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm9sgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1cm8hfv</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>🦋🦋🦋</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cm8hfv</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu May  9 08:09:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_12.xlsx
+++ b/data/2024_05_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C610"/>
+  <dimension ref="A1:C753"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10803,6 +10803,2437 @@
         </is>
       </c>
     </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1cnru64</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>some of my other nails from nails past</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnru64</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1cnrhnm</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">colored frenchies are my fav ever </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fed6zu5jtczc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1cnr4f0</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Freehand Frenchie</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnr4f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1cnqm3a</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Holographic Shimmer</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vaysuo8liczc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1cnq88w</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>The glitter was the right ✨pop✨</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7v8jy3zdczc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1cnpf5e</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>BT Art Box diy</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ebkncjge4czc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1cnoj71</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>3d Nails 😍</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bq9ah2tubzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1cnof7t</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Got (m)y nails done for vacation</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lashy4imtbzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1cnoevr</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Pretty pink just how I like them</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odzwc9hetbzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1cnnjhk</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Got them done recently</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnnjhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1cnnfc3</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Green 💚</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnnfc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1cnnb1g</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Simple honeymoon nails 💕</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnnb1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1cnn7sp</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Shadow Wolf 🐺</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnn7sp</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1cnmvvt</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Rip my baby</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjcx1sapebzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1cnmmni</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>My take at the recent flower nails trend</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnmmni</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1cnmijv</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Fun nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whd3lz5abbzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1cnltsk</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Going to a Tenacious d concert tomorrow and painted these 😆</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnltsk</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1cnljr8</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>My Dad and I did my Builder Gel Fill this week:</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnljr8</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1cnliue</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>just did my first set with the aprés gel-x set</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnliue</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1cnlhoq</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>first press on.. not sure if I like it</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk95zcg32bzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1cnl1ip</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t xml:space="preserve">natural  </t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2fbhdl1yazc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1cnl0ly</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A gorgeous spring set by my nail tech. A purple base with silvery cat eye + teal-ish chrome. </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o134rmfoxazc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1cnknex</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Obsessed with my new set.</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnknex</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1cnjuod</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>New at nail art. Here’s some practice swatches</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnjuod</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1cnjqbq</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Trip to the salon today 🖤💜✨🌙</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnjqbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1cnjoe1</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>How to use these</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnjoe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1cnjnkc</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Mocha nails!</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y37jdq44mazc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1cnjmwx</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Strawberries!!</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygz9swyylazc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1cnjluq</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>fresh set 🥵</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck062u7plazc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1cnj21q</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>hey just a question for anyone who’s a professional that does this</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cnj21q/hey_just_a_question_for_anyone_whos_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1cnicjp</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>decided to try short nails! what do we think?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnicjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1cnhye7</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel manicure w/ extensions </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nap10f88azc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1cnh6gk</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Not bad for $1 press ons</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d7qxh5pa2azc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1cngsf9</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>newest set! ❤️</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cngsf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1cnfajt</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Stickies under nails</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cnfajt/stickies_under_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1cnf7e0</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>💖 sparkles✨</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d6h5uvaun9zc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1cnf3on</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Bloop Bloop</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bewdxn1n9zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1cnes0o</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Peeling, brittle and weak nails. How can I get them looking good and strong?</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bx89jehk9zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1cneh3o</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Most recent set 😌 light pink chrome hard gel overlay on natural nails</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myqflft2i9zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1cne378</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>sailor moon french tipsss</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3lnfi895f9zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1cndki3</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>I just made this set, how long do you think it took me to draw freehand? 🥵😓🤞🏼</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vswbwfjbb9zc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1cnd3wf</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>❤️</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9z78s10s79zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1cncapf</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Thermochromic Liquid Crystal from Major Dijit. I need help!!!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cncapf</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1cnc4zm</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Big gems, big sparkles ✨</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnc4zm</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1cnc47r</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>New Gel X Set</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnc47r</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1cnbydv</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I'm really digging the more nude look stilettos lately</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zbkmt94z8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1cnbm2y</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Clear fake nails on gel?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cnbm2y/clear_fake_nails_on_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1cmuylb</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>How to remove press-on nails safely?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cmuylb/how_to_remove_presson_nails_safely/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1cnbaju</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>press on recommendations?</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cnbaju/press_on_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1cn4tc2</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>First time doing gel nails</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l853i6qmh7zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1cnagxz</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Does anyone know a press on nails brand for large nails?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnagxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1cnao1n</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>She put 4 layers of pink nail polish with some colorful dots and they’re not even really visible 😭</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5p3gytjjp8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1cnahda</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Iced lemonade 🧊🍋</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foxaelk3o8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1cnagfp</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Something different (beginner nail tech)</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qy9g81hwn8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1cnabey</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>love matching my nails to my rings</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnabey</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1cna97s</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>RIP 5 months of growth</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cna97s</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1cna5iw</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kiss Impress modern French in "Snooze". </t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48w60siml8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1cna2na</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Making press ons</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aigibxxzk8zc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1cn9ydg</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Literally obsessed it sparkles so much</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kot7hjf3k8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1cn9sgd</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I love this set 🤩</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsnovqhti8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1cn9712</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Blue and butterflies</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn9712</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1cn7x4b</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Oddities nails… too weird?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrb1stly48zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1cn7b3a</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>What type of fake nails can I apply on damaged nails?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cn7b3a/what_type_of_fake_nails_can_i_apply_on_damaged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1cn74kn</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Gel Nails</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cn74kn/gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1cn6kiu</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>3 months (I think) of growing!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjexoep4v7zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1cn6a43</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>⋆˚࿔ nails 𝜗𝜚˚⋆</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn6a43</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1cn67we</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>nailz 😽</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn67we</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1cn5f9o</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Posting progress.</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn5f9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1cn4srr</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>I finished the other hand 🥳</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvy39kthh7zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1cn45kn</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Recently took these off but these are my fav 🙂‍↕️</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wum6jsy3c7zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1cn3xj1</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>the sequins add a touch of originalit</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cn3xj1/the_sequins_add_a_touch_of_originalit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1cn3gum</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn3gum</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1cn3gs6</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>I like milky but not white!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn3gs6</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1cn3cn2</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loud pink and white French. </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ls0rwm3y47zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1cn39uq</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>I feel like they’re missing something.. help!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yc4mbf3947zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1cn2gj6</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Does this look like terry's nails or normal ? </t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18vpixknw6zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1cn23sj</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Galactic Press Ons from Glamnetic 😍</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn23sj</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1cn1iau</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>My girl always kills it 🔥❤️</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn1iau</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1cn1gqh</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>advice needed!</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn1gqh</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1cn0h7i</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Keeping it short and neat!</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ijvkq36a6zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1cmzqu9</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Which shape looks better on me?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmzqu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1cnqddd</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lavish Lilac </t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlj9plnofczc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1cnp34y</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Can’t get over this intense shift!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnp34y</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1cnombz</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Just my lil’ oranges 🍊</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os31p2oqvbzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1cnn6uu</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Shadow Wolf 🐺</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnn6uu</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1cnn0w9</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Is it obvious that one nail is a press-on?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62fl03fzfbzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1cnmi0f</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">neutral ✨sparklies✨ have my heart </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gk2vvxq3bbzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1cnmemh</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Having fun painting my nails after kicking a nasty picking habit!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsbznh1cabzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1cnlncd</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Removed acrylics, nail damaged, can I put acrylics back on?</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cnlncd/removed_acrylics_nail_damaged_can_i_put_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1cnl0rx</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>essie ink jelly 🖤</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g8s80x0vxazc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1cnkpo4</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>It's On has an unreal glow</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnkpo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1cnjyg0</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Lyn B Designs - Let Life Bloom</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/veqn7mmooazc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1cnjau3</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Rehab</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnjau3</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1cnj472</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>I hope this isn't a stupid question...</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cnj472/i_hope_this_isnt_a_stupid_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1cnifz8</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>So impatient!</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zta7hn24cazc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1cnieco</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Cirque Colors Lucky Bag</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cnieco/cirque_colors_lucky_bag/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1cnc7ou</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Green frost by Belier</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mtqh42rx09zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1cnh2z9</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Regular mail polish similar to dnd purply pink?</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cpqrypk1azc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1cngw37</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>First time using holo</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cngw37</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1cmy5my</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>malicious nail tech…?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cmy5my/malicious_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1cng1v9</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>I think I’m getting better at this</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cng1v9</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1cnfly6</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>SO cool and sparkly! (April PPU)</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnfly6</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1cnfk89</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Sunset on my nails 🌅</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnfk89</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1cneprj</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>EARTHY</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cneprj</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1cnel23</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Making lemonade out of lemons 🍋 💛</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnel23</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1cne7tj</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>This gradient was made using a KITCHEN sponge!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cne7tj</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1cne3ut</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Alchemy lacquers Tristram</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cne3ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1cndxcw</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>I get why this is a fan favorite now</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n9bpwzyd9zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1cnd33k</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>ILNP Fairy Dust as a topper</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y32g2wwl79zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1cncuz0</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Need help with a broken(ish) nail</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cncuz0/need_help_with_a_brokenish_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1cnboyp</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Sassy</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6sq2gs6x8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1cnbhyy</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>so how did they do 💜</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnbhyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1cnaqzh</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>how to prevent gel “lip” post nail growth</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnaqzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1cnager</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>When to use gel base in conjunction with dip powder? Do you ever apply gel base to anything other than your bare nail plate? What about PH Bond? ((What does any of this stuff dooooooo))</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gscnwm7tn8zc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1cnadrr</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>{PR} Current Affairs by KB Shimmer</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ddyscwbn8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1cn9t6c</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>This became an instant favorite!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn9t6c</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1cn9bwn</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>💚 Emerald City Vibes 💚</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn9bwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1cn8z8n</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>I’m enchanted by Enchantment</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lx9pu9irc8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1cn8x18</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Clay cuties</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2w9a7k2bc8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1cn6w11</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Can it please be summer already?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn6w11</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1cn5sr8</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Is there a way to thin out builder gel at home?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cn5sr8/is_there_a_way_to_thin_out_builder_gel_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1cn52mk</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm in love with this color </t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/itpcohnrj7zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1cn3yt2</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Messy but I have to share this shade!</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn3yt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1cn34os</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Looking for a Dupe -- Frenchie Likes To Kiss</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nj5uv0uw27zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1cn2fsi</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Looking for a 2000s nail polish swatch blog</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cn2fsi/looking_for_a_2000s_nail_polish_swatch_blog/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1cnq9mj</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Simple, but delicate :)</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kn1lxvy9eczc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1cnpjp9</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Spooky in Spring</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9tp06qw5czc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1cnojcq</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Closeup before changing the design</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnojcq</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1cno7pi</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Stickers 🌟</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u34giechrbzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1cnlv4c</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Red and Rhinestones</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvihv0if5bzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1cnlunm</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Painted these for my tenacious d concert tomorrow!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnlunm</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1cnjxvr</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>New to nail art and did some practicing</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnjxvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1cnh8jy</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Spongebob!!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l0zxaa1q2azc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1cnf4xv</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Droplet Buddies</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnf4xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1cnf3h4</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>So sparkly! ✨💍✨</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnf3h4</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1cndmvl</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>My spring set DIY hand painted, a holo nail, and some 3D</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cndmvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1cnbuy3</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Birthday nails ✨</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wr98e3dey8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1cn9v76</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>was hoping i could get some good opinions</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn9v76</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1cn9605</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Blue and golden butterflies</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn9605</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1cn8rda</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Butterfly Wings</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn8rda</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1cn8ncz</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>MyMelody Inspo Set!</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo2777kba8zc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1cn3ufz</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Bees &amp; flowers</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cn3ufz</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1cmza8b</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Long nail or short nail ʚ̴̶̷̆ ̫ ʚ̴̶̷̆</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cmza8b</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri May 10 08:08:41 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_12.xlsx
+++ b/data/2024_05_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C753"/>
+  <dimension ref="A1:C906"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13234,6 +13234,2607 @@
         </is>
       </c>
     </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1cok960</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>gel peeling?</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2ziiv1i3kzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1coimom</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Nail not growing properly after surgery</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coimom</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1coidpw</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>first time painting my nails on my own instead of going to salon, sorry if it's messy i tried my best</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8l6sitlagjzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1coicnt</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>best press-on sticking tabs?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1coicnt/best_presson_sticking_tabs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1cohydy</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I got acrylics for the first time! I love it and I'm never going back!</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cohydy</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1coh7d6</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Ombre nails</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coh7d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1coh2a7</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>so i have parakeets and they leave their feathers everywhere. if i were to hypothetically wish to put their feathers into my nails to make them look cool or whatever, would i die? let me know.</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mjc1c6e1jzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1cofr14</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute nails I did </t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccqgc0m3oizc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1cofqdi</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Sharing my favorite sets I've gotten 💖</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cofqdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1cofjr9</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Nail Salon Recommendations</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cofjr9/nail_salon_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1cofdrs</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>natural nail journey of like 3 months gone ;-;</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cofdrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1cof06e</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New sets I made! </t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cof06e</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1coebmy</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Pink with heart set 🩷</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coebmy</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1codznr</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>First Set Help</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1codznr/first_set_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1codye7</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Got them done</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1codye7</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1cody3m</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Got them done</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cody3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1codgkz</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>First french!!</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1codgkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1cod0ki</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Love me a good brown</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nvxjo8glyhzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1cocn6n</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Cotton candy</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aneyqo8bvhzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1cocfj3</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Today’s nails, who love’s it?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qir7jv0gthzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1cobxtp</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>just fell to my knees</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nuhbmy8phzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1cobeep</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got to do some miffy nails today 🫶🏽 </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1mlzlqokhzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1cob0sx</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>{PR} Glowy Jelly Fish Nails</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cob0sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1coapk0</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I finally started a nail course!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coapk0</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1coapi8</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Gel extension and poly gel issues</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6wbov5yehzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1coac4w</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coac4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1coaa9u</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Is this too nude for me??</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coaa9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1coa7sl</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>First attempt at French nails with polygel. I used fake tips and applied polygel over them</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coa7sl</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1coa3yb</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>What long nail hate? 💁🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l30w3179ahzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1coa1ge</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Holding My Work Cup: Ep 9 - Kirby Dream Buffet</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36lrepkp9hzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1co9zdz</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Kiss Press On Nails. First time with Almond shape</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z0im7s299hzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1co9rqh</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Pink French for mamas day 🙋🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lse6wykm7hzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1co9l64</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Practicing</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t5ga38z36hzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1co9l4y</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Told her she can do anything she wants, and she asked how I felt about flowers and pastel...</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co9l4y</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1co8jkx</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Is it normal practice to use a dremel tool on natural nails?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1co8jkx/is_it_normal_practice_to_use_a_dremel_tool_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1co9ghv</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Milky Pink</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsqecui85hzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1cnxtzv</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Gudetama Nail I Tried Making (practice) Reference Photo Last</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnxtzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1cnz6ez</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>UPDATE - the missing element was glitter!</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zkfq2elzezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1co8y4d</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Mermaid nails 🧜🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0heymo91hzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1co8ukd</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>My nail beds are extremely flat, is it possible to reshape them?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1co8ukd/my_nail_beds_are_extremely_flat_is_it_possible_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1co8o68</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Peachy micro glitter </t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxjgor64zgzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1co8fki</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Enjoying sunny days in the uk ☀️🍉</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmxekfi9xgzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1co160r</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>I painted these nails inspired by Iso from Valorant 💜</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp3xcpdrefzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1co332f</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">how to protect best </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1co332f/how_to_protect_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1co3n6p</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>First time getting designed nails</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q53352ipxfzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1co81gb</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Broken nail</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yx4jzavbugzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1co7xcz</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Why are certain areas holding gel and others are peeling? (Check comments for more information.)</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d73mnh2itgzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1co7rfb</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>About longer lengths</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1co7rfb/about_longer_lengths/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1co6vfo</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Simply bubblegum</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egprunynlgzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1co6iou</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Short white nails always give me chiclet vibes 🤍🤍</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0g2ash92jgzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1co64kq</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Nail health?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/taa1sd66ggzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1co54lk</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>2nd time polygel!!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co54lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1co4pxx</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>These remind me of those stars I always wanted to put on my ceiling🤩</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/20igry5n5gzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1co3z2k</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Just noticed that Cutepolish designs from 2012 are coming back into trend. Partly the checkers and the cat eye metalic polish. Anything else you've noticed coming back into fashion?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1co3z2k/just_noticed_that_cutepolish_designs_from_2012/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1co3py3</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Feeling....koi</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co3py3</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1co3add</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Has anyone tried Young Nails/Dip Powder recommendation?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iggwzb35vfzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1co37by</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>nail polish will not stick</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xab6m9whufzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1co2wx4</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Beginner Nail Artist</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co2wx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1co2p8e</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>I don't know why but I don't feel so comfortable with square nails anymore.</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5z4v8rygqfzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1co20u6</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Did some press ons!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co20u6</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1co19i5</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>OPI in Scorpio Seduction 💙</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co19i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1co08jk</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape would look good on my hands? </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co08jk</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1cnzlq8</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>cat eye gradient :&gt;</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4tykr9u2fzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1cnzirc</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Cleaned my husbands nails 🥰</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnzirc</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1cnz1g2</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>love a good pink!!</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0bmb3i3jyezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1cnyz4r</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Not sure what’s going on with my cuticle, it always grows back no matter how I try to get rid of it</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgbcr22zxezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1cnysiw</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Strawberry Shortcake Vibes for Spring</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdjr4jwiwezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1cnyb4g</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>I found my favorite set!</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnyb4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1cny2e9</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>obsessed is an understatement 🩷✨</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cny2e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1cny214</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neon, gothic punk. </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qo3tm4qmqezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1cnxlcp</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Just my own, short nails after having press ons for months</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt814vpxmezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1cnxd1a</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Mashup nails xD</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y09pd8iykezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1cnxaeo</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>New Nails and Natural Nail growth!</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suxlcsqckezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1cnx4bi</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Nude bling ✨💖</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tf19fa1yiezc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1cnwrz6</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>How is this effect created?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xx9759h2gezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1cnwl7i</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>struggling to grow out my nails when they continue to bend upward. what can I do to stop this?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnwl7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1cnvhho</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's my very first time doing m'y nails can i get some advice please </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1htqlbke4ezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1cnv8vq</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Pink textured nail art</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnv8vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1cnv6e9</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>My abstract version of watermelon nails</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eo4rh1he1ezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1cnv4gk</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Testing my new Mooncat polish</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kq4lbmv0ezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1cnugy7</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Simpson Nails!</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnugy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1cnu4w5</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Applying polish for the first time </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyh9hidkqdzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1cntucz</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Need help with weak nails</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91w67yc6ndzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1cntssk</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Forever in Love With Red💋❤️</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cntssk</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1cnrzw8</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>OPI-I Think In Pink</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnrzw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1cnrzeb</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Broadway Colors-Summer Bikini</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnrzeb</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1cojxga</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>I’m always going blue</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k75med4dzjzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1coijr9</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>wet-looking top coat recs!!!</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1coijr9/wetlooking_top_coat_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1cojr4d</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>SpongeBob nails</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cojr4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1cois6z</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>accidentally perfectly matched my kindle</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmbzm030ljzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1coidrb</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Did my sil’s nails💅 a bit of a flower/sun theme☀️</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ujpw8cbgjzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1coibye</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Dark Heart</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coibye</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1coh1po</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>LOVEEE sparkly pink nails</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coh1po</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1cogt4e</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some unsexy, just doing stuff you gotta do, pics of my very pretty new Holo Taco polishes </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cogt4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1cogk7h</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Amazing </t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2puqcj56wizc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1cog3mo</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>My cat thinks my claws could be sharper 💅🐈</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3d9eofglrizc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1coebap</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Cirque jellies 🥹</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coebap</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1codp9y</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Absolutely RIDICULIUS nail stickers came in the mail today</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjvmgbgr4izc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1cocuoo</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Sally Hansen [ Insta-Dri]  shade: On The Download</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5yea0tv5xhzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1co9fub</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Getting so much inspo from this subreddit!</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/go705pm35hzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1cobqns</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Chicago Fire 🔥</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cobqns</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1cobiuh</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>First time using Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cobiuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1cob6hu</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Mourn with me: Recently moved, finally got to hang my polish racks... Promptly dropped my brand new, unopened bottle of Turbocharged 😭 Then noticed it was somehow bottled into a Glass Candy bottle?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cob6hu</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1coaxvj</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Shimmy Shake</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coaxvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1coao1j</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Starrily Amulet or Cirque Chemistry?</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coao1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1co88si</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Nail shape advice</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co88si</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1co5sxp</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>A red I actually like 🤎</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co5sxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1co5m4h</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Did my nails yesterday and wanted to share</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co5m4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1co5gwg</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Subtle pink blobs on shorties!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vokby21bgzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1co4v1w</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>New tech appointment in 2 weeks for gel and potential art on my VERY short natural nails. I can't decide on art. What is a simple, trendy style I can do for Almond with nude near my cuticle so it can grow out more naturally / allow infill ?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1co4v1w/new_tech_appointment_in_2_weeks_for_gel_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1co4hyl</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Summer vibes</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/auyy92004gzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1co49rq</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Love it - Noite de Gala Colorama</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0krl5s62gzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1co3f1f</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You made me buy Bluebell and I have no regrets. </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjnuwa13wfzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1co2xq6</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Prefer Pink? Pick a plethora!</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkdn7unesfzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1co2owb</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Baby blue nails in nature</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co2owb</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1co2fnh</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Dark brown - Masha's Gel Polish</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7ja72aaofzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1co2f5h</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 order VIA phone - SUCCESS!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1co2f5h/nailtiques_formula_2_order_via_phone_success/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1co23j0</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Color4nails order issues</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1co23j0/color4nails_order_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1co1v4g</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Till the Music Stops</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x1gbase6kfzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1co1bpt</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes a nude needs some sparkle ✨️ </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhlbso80gfzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1co1bcz</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Pink Jelly</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1co1bcz/pink_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1co1akn</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Obsessed with this color palette 💚🩷💜</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vaezpm4rffzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1co1afp</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>besties 💙🔥</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co1afp</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1co1007</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Swatch Comparison Request: Penelope Luz - Tendresse vs. Mooncat - Mermaid Bait</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1co1007/swatch_comparison_request_penelope_luz_tendresse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1co0urz</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Koi pond 🐠</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co0urz</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1co0ee6</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First attempt at modern art nails. </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biipjbo09fzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1co0479</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Happy Europapa day!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wf09s70s6fzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1cnz4h2</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>In which I eat crow</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c635qdd5zezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1cnysgd</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>It's giving Shrek vibes</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22w56whhwezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1cnyaen</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So forgiving and beautiful </t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/it8cakdhsezc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1cnxo8s</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Looking for a dupe</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzq3jc8mnezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1cnx6o4</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Essie - Mint Candy Apple</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h59bsa1hjezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1cnwwpv</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>12 day wear on everyone’s favorite polish✨</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8k885cz5hezc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1cnvyjw</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>So shiny ✨</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnvyjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1cnum3v</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Mall Crawler and so what if I’m just putting it on everything now…</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnum3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1cntxnl</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Starting to appreciate short nails, even though it makes my sausage fingers look less feminine. Just grabbed this polish from a charity shop, Barry M coconut infusion "Oasis". Cheap but pretty</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cntxnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1cnt7z0</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>20 minutes after boarding a plane smh</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnt7z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1cnsac7</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>In love with Holo Taco’s Teal No Lies</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnsac7</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1cok3yf</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>Azulejo/Deltware Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s50h4r9p1kzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1cojsnw</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>I love my simple nails, but with style.</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7xyw56nxjzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1coi6oe</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Good morning 3d gel and a straw</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1gj2lq1ejzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1cofkax</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Oooh you give me butterflies😍🦋🦋 set by mee 🥰</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/diddsk59mizc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1cofjil</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Matte &amp; glossy French manicure help</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cofjil/matte_glossy_french_manicure_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1co8ima</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co8ima</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1co555k</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Feeling... koi</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co555k</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1co534l</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>First spring nails</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co534l</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1co4y4m</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Ursula Inspired</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wzhyoed7gzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1co4qys</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>These remind me of those stars I always wanted to put on my ceiling🤩</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tcu0gosu5gzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1co2y1p</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>My nails for 90s theme party</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1co2y1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1co13q7</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Anyone knows how to make this?</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1co13q7/anyone_knows_how_to_make_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1cnztpg</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Did my nails again!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/86wafwvi4fzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1cnxsh6</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Tried making Gudetama Nail (practice) Reference Photo Last</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnxsh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1cnwtiu</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Spring Nails</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cnwtiu</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat May 11 08:07:28 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_12.xlsx
+++ b/data/2024_05_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C906"/>
+  <dimension ref="A1:C1082"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15835,6 +15835,2998 @@
         </is>
       </c>
     </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1cpb64s</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My bf mad me mad so I’m going to paint his toenails in his sleep </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpb64s/my_bf_mad_me_mad_so_im_going_to_paint_his/</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1cpb5cm</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>do I just have abnormal nails?</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f2l77mitqzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1cp9zgc</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Most durable DIY</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp9zgc/most_durable_diy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1cp9tzy</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>☄️</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5zo2zrceqzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1cp9to6</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Keep brushed on powder nails or switch to Gel of some type?</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp9to6/keep_brushed_on_powder_nails_or_switch_to_gel_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1cp92zn</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Light pink with white chrome</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xq59q1y5qzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1cp8ro0</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I asked my manicurist to give me a galactic effect that was not exaggerated </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3netk9ll2qzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1cp8oa5</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Damaged nails. Need advice</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp8oa5/damaged_nails_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1cp8myk</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Soon it will be recycled into something new, but I can't reveal it yet</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pbhuz4y51qzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1cp8m40</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>i got my nails done for the first time today, they’re pretty bad quality.</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/78xjkup01qzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1cp8gak</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>What exactly is bio-gel &amp; was my experience normal ?</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp8gak/what_exactly_is_biogel_was_my_experience_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1cp8fum</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>spring nails 🌿🌸</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp8fum</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1cp82wj</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Love 💅😍</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp82wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1cp7tac</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Tortoiseshell Nails</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp7tac</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1cp76eu</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Water drops</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp76eu</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1cp75nm</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I'm a fan of this color combination.</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp75nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1cp6sw3</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>had to repost my strawberry nails cuz i got way better pictures 😅🍓</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp6sw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1cp61kc</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>What do you all think of my latest cat eye nails?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bqnqj6sbpzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1cp5p7e</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Pink Aura Nails</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87qpsb1k8pzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1cp5mlk</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>A little bit of spring</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bv61il3v7pzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1cp564x</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>got my nails did for some self-care today, first time in almost a year!!</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp564x</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1cp4xuz</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Evil eye set 🧿</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unyplj8l1pzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1cp4pbc</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Doing my own nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp4pbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1cp4oip</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Is extensions/builder gel possible?</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtylxnq6zozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1cp458r</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Friday evening mani w/ my wife I did french &amp; she did like creamy? ☺️</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6v3fyqduozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1cp398w</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>I miss this set so much</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/quag2k3smozc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1cp323g</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Dipping powder polish?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp323g/dipping_powder_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1cp31ho</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Gel polish brands?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp31ho/gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1cp2vzp</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Beginner DIY (full coverage tips, gel glue)</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfj38lnrjozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1cp2h0m</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vacay Nails! They’re giving Barbie, I love them 💖 </t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jknc86jgozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1cp28uh</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Plain nails with top coat 😍</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp28uh</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1cp1ypz</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Gel manicure, input needed</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bqhyz0lcozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1cp1ydb</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails! 🍩 First time doing DIY gel extensions, any tips for tackling the seepage around the edges before the glue cures? </t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah5jfvricozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1cp1nue</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>What do y’all do when you get your nails done and end up hating the color that you picked?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jaw9ci3aaozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1cp1kp7</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Pink magnolias 💖</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp1kp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1cp1jm6</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Did them myself, it's semi permanent nail polish (uv). What do you think?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp1jm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1cp1il9</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Nails 💅 Yey or Ney?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9huc4w39ozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1cp1feq</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Loving this abstract design</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4cr2vxof8ozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1cp18de</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long time BIAB user, wanting to switch to press-on nails </t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp18de/long_time_biab_user_wanting_to_switch_to_presson/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1cp114d</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Thank you!</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp114d/thank_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1cp0ytg</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>First time going out with my nails done</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6brx3ahx4ozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1cp0xi7</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Gummy nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cp0xi7/gummy_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1cp0vp5</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Which nails should i do</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jafa3u594ozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1cp0a5e</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Repost #NailArt</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5soki0eoznzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1cp07cj</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>What are these giving?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e4bg6d56znzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1cp031y</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Rainbow glittery fluted glass nails by me. The holo glitter really shows up in the sun!</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp031y</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1cozr74</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a little simple 💎 </t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywhk2zurvnzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1cozq1o</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>I'm not quite ready for winter to be over. ^-^;</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cozq1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1cowgag</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Cotton candy inspired nails 🩵🩷✨</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cowgag</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1cox0l9</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Do not buy! 🩷</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cox0l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1cox5ho</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Long nail girlies: how do you do these things??</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cox5ho/long_nail_girlies_how_do_you_do_these_things/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1cozjcp</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Spring nails 💜🪻</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cozjcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1cozbkr</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sunflower Nails </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lsm4u5ijsnzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1coz459</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Press on nails?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1coz459/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1coxfqq</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Tried a full magnetic mani for the first time; took forever! 🤣</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dedbk66enzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1cowwc0</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>New nails. Who dis?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cowwc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1cowh6h</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>First time doing nails, how do they look?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iub89x9x6nzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1cowa6k</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Vacation nails!</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cowa6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1cow3jx</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Much needed manicure.</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zl699rr04nzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1covxes</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Summer Vibes</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1covxes</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1covt86</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>I’m trying to get better at nail art</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1covt86</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1covdlk</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Some starry night nails for you.</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyk64gnfymzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1cov8tv</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Galaxy Nails</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cov8tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1cov41b</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Blue Nails</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg73v2ubwmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1cov22c</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Just did my nails 🥰 thoughts?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cov22c</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1coumxs</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>dark green base and light green cat eye 🐍</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coumxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1couhng</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Matte top coat</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1couhng/matte_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1cotykb</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Gel x cat eye</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cotykb</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1coty5w</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coty5w</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1cotxwc</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Nails I did yesterday, do you prefer square or almond??? 💅</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ub0gvlngnmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1cotwnq</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Birthday cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3apjq06nmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1cotw29</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>My go to nail polish</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3u56ikg2nmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1cot97d</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying the gel x </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cot97d</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1coson1</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>My natural nails. Is it possible to straighten out the one that grows straight down and crooked?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coson1</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1coskrt</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>To all those who told me to get almond…i made the leap</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwpqhyh3dmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1cosid4</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>I really need help! I dont know what to do:(</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cosid4</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1cosglm</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>☁️⛓️💫</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3oy51n5cmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1cosfk6</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>My poor nail artists have to work with mini nails🥹 You girls with long nails, tell me how are you so good at this!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nrctmr0cmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1coscsb</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Red nails</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coscsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1cosbih</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Does this colour wash me out, I want to make pastels work so bad !!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uwloqha5bmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1cos4y5</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>What can I do better?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cos4y5</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1cos255</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Happy Little Clouds</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6vvhpg49mzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1corzmx</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>8th DIY</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1corzmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1corwn7</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1corwn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1coro46</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>I love to draw but nail art is unexpectedly difficult!</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coro46</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1cor9ea</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>I love the chrome!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/050da1013mzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1coquxw</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Nail tech did gel x and they look like this</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvsqd76vzlzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1coqsmc</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Summer vibes💚</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5x5uv0dzlzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1coqjyd</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Heart attempt 💗</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coqjyd</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1coqe2w</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Hi, I usually go with oval nails shape, but i kinda want something different. What would be your recommendation? Would coffin one look good? Pls help</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lwo5ez3wlzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1coq5mh</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red is always a classic. Which look is better on my nails? Square and matte or almond and shiny? </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coq5mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1copzah</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>I love doing gradient to transparent !</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sisff13uslzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1copu14</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Mother’s Day nails</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58kt3ibnrlzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1copsm2</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>What was used on my nails? Help!</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/961vt03brlzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1cop2i4</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>I’ve been very happy with my new nail tech 💕</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rfx5qmg1llzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1cop1x9</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>I like this shade of pink 💗💅🏻</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cop1x9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1cop1tf</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>New 🆕 set tropical 🌴</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1eguv7vklzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1coowhq</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which pink is better??? </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coowhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1coov8b</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>My new set of my</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zr4rsyf9jlzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1coo8au</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>I have chubby fingers/hands. Can almond shape look good on my nails?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coo8au</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1cpbt94</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Sheer Fantasy</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpbt94</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1cpadoy</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Some recent press on sets that make my heart skip a beat</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpadoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1cpa826</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>🐦‍⬛ 💠 I’m Through Running Away ❇️ 🐦‍⬛</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9d5afsktiqzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1cp9jm1</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>CND Solar Oil reformulation?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cp9jm1/cnd_solar_oil_reformulation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1cp94r2</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>So so sad 😩</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xeh6mihh6qzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1cp8khp</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>I blame all of you!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cp8khp/i_blame_all_of_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1cp7etn</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>A visitor to help me model</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp7etn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1cp7b73</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Can I add the OPI polish thinner to this?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m5izprurnpzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1cp649r</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>It might be time to put the kibosh on the color blue 🤡😂</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6cmy92icpzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1cp5zuu</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>22lb magnet</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cp5zuu/22lb_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1cp5u11</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Pink Aura Nails</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp5u11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1cp53h0</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Best decision in awhile</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp53h0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1cp4pp4</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Clean Up Brush</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cp4pp4/clean_up_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1cp4ir1</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>✨🦖THE GREENS 🦖✨</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp4ir1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1cp3rwo</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>In search of a dupe for 'Tangerine'</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43x8rzz8rozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1coz2fd</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Sultry berry creme (plus cat and mani inspo pics)</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coz2fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1cp3ewk</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Restored an old Illamasqua bottle!</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp3ewk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1cp3deg</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Dog tax Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp3deg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1cp2x0k</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Would love to get this look-what is it??</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ifdavlzjozc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1cp2sxk</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>The best part of coming home from vacation is knowing you have nail mail waiting for you! 🌷💕🌸</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjkr1v05jozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1cp2g7v</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Mooncat magnetic polish not drying after hours?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/guem1w5dgozc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1cp1oyp</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Cuticle Oil Pens recommendations?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cp1oyp/cuticle_oil_pens_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1cp0wi8</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Can you help me narrow down my next Mooncat order?</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp0wi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1cp0azo</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Fluted glass glittery holo chrome nails by me. They look so different in different lighting 🌈</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp0azo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1cozy1i</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>{PR} Mix it Up &amp; Scratch That by KB Shimmer with flash</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rb1c7sx8xnzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1cozxzl</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>Daisy Chain Polish skittle!</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxp6xlg8xnzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1cozrnw</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Help me quit gel PLEASE</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cozrnw/help_me_quit_gel_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1coznzs</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Manicure ideas wanted! Short nails for rap concert</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1coznzs/manicure_ideas_wanted_short_nails_for_rap_concert/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1cozi0c</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was influenced by this sub and I regret nothing </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am3gxhkwtnzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1coysew</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Blood Moon 🩸🌙</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coysew</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1coymqu</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>✨willow (ILNP’s version) (ft. DVN)✨</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coymqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1coygu9</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Only been wearing Mooncat the past month 💫</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coygu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1coyb3h</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>This shade is chaotic and I love it</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coyb3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1coy6u9</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Friday crackle mani (ft shorty middle nail that I broke opening the fridge)</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coy6u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1coy32c</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>PPU Rewind - what colors do you want to see?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coy32c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1coxlm9</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>I found these beauties for $1.50ea at Five Below</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coxlm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1coxgfq</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Tried a full magnetic mani for the first time; took forever! 🤣</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlwuqzsbenzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1cooj1j</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Any non-gel polishes like this?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sv097gk5glzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1cox5qk</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Finally did a summer mani!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwllz543cnzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1cowkwg</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>LynB Witch's Ball</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3d30ual7nzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1cowfix</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Working on my nail art. Super new to it and my lines need work but it’s a start!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zo1lc5xj6nzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1cowe1y</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Jade jelly 💚 my first cirque jelly and I think I’m in love</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cowe1y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1cow59h</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>SeasideKingdom feat. Pitstop</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02wikxfe4nzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1covemh</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>ILNP Teddy velvet manicure</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1covemh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1covazy</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Magnetic Space Play</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/se1lh8evxmzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1coutae</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>I feel like this color doesn't go well with my skin tone but it's such a lovely pink</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coutae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1couqlf</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Trying to get the last of the sunlight to take pictures of spyglass by Holo taco</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1couqlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1cougjq</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Spring sparkle gradient</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cougjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1coty7t</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Ghost Rose or Siren from Cirque Colors?</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r39j95djnmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1cotwvt</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Is it purple? Blue? Shimmery goodness??</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mszrris8nmzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1cotq4s</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>My manicure is so pretty I feel like crying</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cotq4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1cotbl6</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>I used to be a nail biter</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g65guiqimzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1cosp8o</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Saw this color posted here and had to try it myself ✨</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cosp8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1coshu8</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Maelstrom by mooncat might be the most beautiful polish I’ve ever used</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coshu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1cos32v</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*faceplam* </t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cos32v/faceplam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1corsjt</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Minty gradient </t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvl6t0u27mzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1cormc0</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Mooncat Similars</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cormc0/mooncat_similars/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1coptwd</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>I was just gonna buy one!</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1coptwd/i_was_just_gonna_buy_one/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1coprd1</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Farmer’s Mums</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coprd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1cophif</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Station lighting ✨</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u7s5uzoolzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1cooye8</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>My magnetic set up in action 💚</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/57ojb4wxjlzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1comukq</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>First attempt at gel nails!</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1comukq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1comcl7</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Diamonds💎</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ae2zvhsytkzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1cp7iac</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>My top 10 favorite set! IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikjc7ceqppzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1cp7enp</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Freestyle set. How I do?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u91h1nepopzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1cp755x</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Witchy Nails ✨🌙</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp755x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1cp61hw</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>I did a little nail art :3</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp61hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1cp2l27</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Cute carrot nails</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp2l27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1cp2j25</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp2j25</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1cp0915</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Fluted glass glittery holo chrome 🌈</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp0915</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1coz16k</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>I did these nails a couple of months ago, I want to look elegant, should I choose this design or baby boomer?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1coz16k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1cowdxf</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Just me a nail art novice, practicing!</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/91vxd3z76nzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1couvsh</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Ice cream nails 🍨</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pg4wqexlumzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1cosssc</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Can I paint over gel x and acrylics?</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1cosssc/can_i_paint_over_gel_x_and_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1corkk6</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Bugs 🪲</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1corkk6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1cooo07</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which pink look is better? </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cooo07</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun May 12 08:08:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_05_12.xlsx
+++ b/data/2024_05_12.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1082"/>
+  <dimension ref="A1:C1243"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18827,6 +18827,2743 @@
         </is>
       </c>
     </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1cq2pth</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love glitter </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kvzglh6acyzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1cq29kf</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Caramel latte nails </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtmzb1ah6yzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1cq1qka</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Does anyone else have trouble getting yellow gel polishes to cure??</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cq1qka/does_anyone_else_have_trouble_getting_yellow_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1cq1gbd</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Prom nails for a friend!</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cq1gbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1cq15ep</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>I did it too :)</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cq15ep/i_did_it_too/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1cq11pn</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted my girlfriend's nails tonight! </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ab37m6arxzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1cq0xwj</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>My sister did my nails!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw2ep510qxzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1cq0vdv</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>3 sets i did today</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cq0vdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1cpygq4</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Looking for colors that give the see through jelly effect</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m0zp6ybgywzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1cpy9ek</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Mooncat Sale</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpy9ek/mooncat_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1cpy3fd</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Girls, what do you think of this type of nails? I got bored with making extravagant designs and I wanted to make something simpler like this😅🥹</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g14qxy6ruwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1cpy1rr</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Next trip isn't for another 3 months, but this color makes me feel Iike I'm on vacation! </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qizu9ky9uwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1cpxqoh</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>these were meant to be crazy-unusual, but i fear that they’re just bad-unusual. opinions? (two pictures)</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpxqoh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1cpxpwi</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Felt like trying something fun</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2tr87v8uqwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1cpx7ot</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Got my nails done to match those of my Cyberpunk 2077 character</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4l9wmtulwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1cpx1ut</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>I love a short almond 🥺 Nexgen dip on real nails</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2egnak8kwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1cpwoox</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Poly gel broke, so I got a gel manicure after removing the poly </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1wyyqslgwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1cpwkp8</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Hello Kitty Pink!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra56hb1ifwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1cpwfp6</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Y’all I’m starting to think I can really do this</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cfado1u4ewzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1cpuxhh</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Olive and June Press On Warning</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpuxhh/olive_and_june_press_on_warning/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1cpv409</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>I’m in love 😍</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpv409</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1cpv87x</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Is this as bad as it feels?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g2uob7p2wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1cpvmhc</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND 267 🌸 </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0y7i7kc6wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1cpvl24</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Bingata blues</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5ouzsk06wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1cpv66k</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>press ons from two weeks ago 🌸💕🎀</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1362ee172wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1cpuvrb</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Fresh Set</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13mf8i7jzvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1cptwti</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Periwinkle base with some water decals</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cptwti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1cptt4p</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue with some sparkle! ✨ </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc5l8h92qvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1cptlp5</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>soft gel or hard gel?</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cptlp5/soft_gel_or_hard_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1cptl6y</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Two days over 65 degrees and I have officially switched into summer mode 🌈🩵🧡💚💙</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ca2wpwc7ovzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1cpsuv4</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Chrome nails nightmare</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpsuv4/chrome_nails_nightmare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1cpsp4o</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Fun little set I’m calling Tequila Sunrise 🌺</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7sfso4yjgvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1cpso4y</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Thoughts on these, not sure how I feel about them.</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/meqwr6hbgvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1cpsdnt</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>More nail art! This is fun</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/832v4s5udvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1cprftt</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">obsessed with this color </t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygut3m6u5vzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1cpqxf4</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Color swatching</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a060xljj1vzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1cpqs1x</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else's posts keep getting deleted? </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpqs1x/anyone_elses_posts_keep_getting_deleted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1cpqhi4</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>not perfect but i love themmm</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpqhi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1cpqa30</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Mermaid nails for my Master's graduation 🎓</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpqa30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1cpq1jj</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>cute wavy nails!!</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2xhmty0uuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1cppz02</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Lemons!</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyr7v5nftuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1cpptrv</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>After a year of ignoring my supplies due to stress, I finally pushed myself to make my first pair of press ons today!</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8v8z26asuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1cpppop</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Don't let friends paint your nails </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1eah7cbruzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1cppeur</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>They are a bit outgrown but this is one of my fav sets I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15g5ysxqouzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1cppbrr</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Le's Nail Salon &amp; Spa</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2clyay2ouzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1cpp13a</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>10 Romantic Valentine's Day Nail Art Ideas You'll Love</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzk7z42gluzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1cpopmi</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>🎀🐇🩷💗💓✨</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpopmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1cpoo63</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Pink / purple gradient cat eye with iridescent powder on top 🥰 Pics don’t even do them justice!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpoo63</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1cpokk8</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>First time using gel!</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpokk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1cpns24</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/te3wizc4buzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1cpnmbu</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>I love my French classics 😍</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m20ast6r9uzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1cpneln</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>First acrylic set🥹</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpneln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1cpn7bk</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Obsessed with my new nail artist! 🥰</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an5t11qc6uzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1cpn36t</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>First time getting French and im in love!</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpn36t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1cpmpvv</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wwyd </t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpmpvv/wwyd/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1cpmoch</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>French set</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpmoch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1cpm60r</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Aurora nails ☺️</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51ufiktlxtzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1cpm5n4</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Pre cleanup, but man, I love this polish!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vg3n5mixtzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1cpm23w</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>pearl nails with 3D designs!🌸🎀</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpm23w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1cplrkh</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Nails in Exeter uk</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cplrkh/nails_in_exeter_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1cpllrx</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>My first ever acrylic nails :D</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1wfl2k0ttzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1cplcx3</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>testing out engagement nails 🤓</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cplcx3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1cplbn5</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Press ons of the week</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cplbn5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1cpl3sz</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Rainbow fish vibes</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9s13fs4wotzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1cpl0cq</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Nail advice! Nails look weird</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jezdi0q4otzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1cpkx44</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Jumping on this trend, absolutely obsessed with my fairy wings</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg2ug6jentzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1cpkv8p</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Blue chrome with some gold star bursts ✨</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4ji09tzmtzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1cpkd8i</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with paper thin nails </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpkd8i/help_with_paper_thin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1cpkpaz</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nails fixed</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpkpaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1cpkk9s</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Went to get nail fixed and she made it worse 😭</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1cpkk9s/went_to_get_nail_fixed_and_she_made_it_worse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1cpju1z</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Classic Reds</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpju1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1cpjhd9</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Digging how subtle these press-ons turned out.</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ozeyc5ebtzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1cpj17k</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Birthday nails!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z779g5mm7tzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1cpiuol</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Elegant and simple</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg5s6fh26tzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1cpirmc</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>I loved my nails.</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gte15f5d5tzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1cpijjc</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Tried my hand at some marble today!</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/afvapeof3tzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1cpijey</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Don't usually post but really love these.</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpijey</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1cpi6id</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>How beautiful are these?!!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bt0jdbeb0tzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1cpi46e</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried doing an ombre using pigments, and I absolutely love it </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9snrxeftzszc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1cphz6x</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Did it on myself</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ye9w09fkyszc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1cpgsis</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summer nails </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy3re2eenszc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1cpgff4</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Tried multicolour first time</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7nbiuqujszc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1cpfpam</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Cherries and hearts are my favorite here</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdv0a35j5szc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1cpdmis</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Got nail extensions for the first time! Is it just me or are they not supposed to slope up? (Gel X)</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wv5pbg0orzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1cpdbie</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Progress!</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpdbie</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1cpd7e8</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Is it possible to fix how my ring finger nail looks? It's pressed down on the side because of the way I hold my pencil.</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lk2h3lqiirzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1cpd138</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>white set (repost) 🤍</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpd138</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1cq2ns1</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Did my 91yr old MIL’s nails for Mother’s Day - first manicure she’s ever had!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9exw0vfjbyzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1cq0xsy</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>problem with gel top coat lifting and then peeling off?</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cq0xsy/problem_with_gel_top_coat_lifting_and_then/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1cq0vlu</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Flowers for Mother's Day</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cq0vlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1cq0lsh</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Cirque Jelly Polish Question</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cq0lsh/cirque_jelly_polish_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1cpwvr6</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Mooncat: Mercury's Tears</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpwvr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1cpvthk</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Any nurses with advice on how to make your mani last?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eu9ck4f78wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1cpz0la</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Discussion: thoughts on DND’s release of a “new” line (DIVA)? </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpz0la/discussion_thoughts_on_dnds_release_of_a_new_line/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1cppx4m</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>How to ask for this?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5e3837k0tuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1cpnsyg</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Dupe for Discontinued Star Glitter Nail Polish?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5owi51cbuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1cpxquf</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>flower milk bath</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpxquf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1cpxkjc</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Magnet Polish Questions</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpxkjc/magnet_polish_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1cpxfua</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>First time water marbling!!</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpxfua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1cpx5zd</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>What’s your fave no smear top coat?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r4doirclwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1cpwag4</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Lost your touch by Emily de Molly 🌸</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpwag4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1cpvsol</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Can you help me label my like 10 y/o nail polish?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/av4ql92t6wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1cpptvc</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>ILNP Songbird</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpptvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1cpvokv</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>My new favorite topper❤️ Show me yours!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpvokv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1cpvk8d</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Which shape suits me best? Square, round, or somewhere in between?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpvk8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1cpv6hu</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Emily de Molly never disappoints!</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7p460v92wzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1cpudmj</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>What’s your favorite drugstore black polish?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpudmj/whats_your_favorite_drugstore_black_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1cpubc3</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Nails as Therapy 🍒</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpubc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1cptynx</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’m still learning how to paint my nails, but I got my first order of Mooncat yesterday and I’m in love. </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xhkrbjdrvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1cptju6</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Can't figure out magnetic cats eye</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cptju6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1cpthx4</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Kraft + Songbird</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a868hlkfnvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1cps2lz</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Bésame Victory Red</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g5bh30b8bvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1cpry8b</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>How do you get your mani to last 2 weeks?</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpry8b/how_do_you_get_your_mani_to_last_2_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1cprw5u</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Sparkly Goodness ✨</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cprw5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1cprulk</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>I love a good ghostly polish</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wj8qatic9vzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1cpr0xf</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Nail Mail!</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpr0xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1cpqxo3</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>A Most Destructive Fear</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ensoze5k1vzc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1cpqb0x</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Love a good thermal "gradient"</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnwn4ji9wuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1cpq6lc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>I really like yellow and green nail polish, but…</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpq6lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1cppv4a</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Finally able to do my nails again</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cppv4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1cpptw0</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>I know I need to clean around the toenail better, but how else can I improve my gel pedi?</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpptw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1cpptdq</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>I Can Fix Him</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpptdq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1cpoval</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Mylar Dreams</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzn15ga9kuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1cpopx9</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>A few recent manis ✨️</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpopx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1cpnzw6</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>✨️ Bewitched ✨️</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpnzw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1cpnv09</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Luxio Build help!!!! </t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpnv09/luxio_build_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1cpnohu</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Some Devil’s Ivy in honor of the Mooncat sale!🍃</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1mks8raauzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1cpnc62</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Sunset Dust</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpnc62</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1cpmwmd</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>🍒glazed cherries🍒</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amttym1p3uzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1cpm5nv</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>What did everyone buy from the Mooncat sale?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpm5nv/what_did_everyone_buy_from_the_mooncat_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1cpluef</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm matching with a window </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43rg9h40vtzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1cplrux</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>I have good ideas sometimes ☁️</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cplrux</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1cpljpw</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Twinkly Red 🎀</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpljpw/twinkly_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1cpkw0n</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Belated April Shower Manis</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpkw0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1cpkv42</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>strawberry kiwi therapy mani</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpkv42</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1cpjzmp</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Best brand(s) for thermals?</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpjzmp/best_brands_for_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1cpikx6</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Thanks all for the lovely comments on my last post 🥹 here's more of my short nails, I love this colour but it's so streaky 🥲 featuring my magic potion isopods because why not</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpikx6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1cpigpk</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Show Me Your Eurovision Nails!</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i284h1xq2tzc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1cpigek</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>One month into doing my nails</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpigek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1cphth3</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Bridal Magnetic nails?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cphth3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1cphsws</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'll wear brown in spring if I want to! </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd4wh6czwszc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1cphroe</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>ILNP Vaporwave</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cphroe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1cp4e3n</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>✨️🌈Rainbow Sparkle🌈✨️</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp4e3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1cp7m2l</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Polish advice for neutral skin tones?</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cp7m2l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1cperxy</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Beetle carapace nails - BKL's QoR</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cperxy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1cpefu2</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Sistaco</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpefu2/sistaco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1cpdkhv</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>I love peaches 🍑</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpdkhv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1cpd3nc</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two topcoats </t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1cpd3nc/two_topcoats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1cq1uf1</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>My spring set 🌸</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcin98x41yzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1cq0ffe</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Let’s see how long this charm stays on!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uy4map8vjxzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1cpx5k4</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Nail art I got to match my Cyberpunk 2077 character</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcxkcbm8lwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1cpw9d1</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Make it ✨BLUE✨chrome🦋💙🐳🌀🦕🫐</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4c2e00jecwzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1cpv8cw</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>This was the hardest and most stressful set ever 😢</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1cpv8cw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1cpss5h</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Frenchies with a twist</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujaz4ss9hvzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1cpseqw</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Practiced some more!</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lo8hmcs2evzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1cpqrj1</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mother's Day set for my mom </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6gij2q40vzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1cpqd08</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Some hearts 💕</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f03ihdspwuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1cppyzd</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Summer set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nftq6jkftuzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1cpmz8i</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Cloudy foggy mood</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzpv03ff4uzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1cpjs9c</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Latest nail art. </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ayw0wkydtzc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1cpfve6</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>My last « training set »</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zw3e11p9eszc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>